<commit_message>
feat(develop-local): optimizacion de codigo
</commit_message>
<xml_diff>
--- a/static/templates_base_financiera/5 PRUEBAS SUSTANTIVAS/1 CAJA Y BANCOS/2 SUMARIA CAJAS Y BANCOS.xlsx
+++ b/static/templates_base_financiera/5 PRUEBAS SUSTANTIVAS/1 CAJA Y BANCOS/2 SUMARIA CAJAS Y BANCOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\documentos\Area de trabajo\JVSERVER\ClienteAuditaPro1\sistema-audita\static\templates_base_financiera\5 PRUEBAS SUSTANTIVAS\1 CAJA Y BANCOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\documentos\Area de trabajo\JVSERVER\Desarrollos-Clientes\ClienteAuditaPro1\sistema-audita\static\templates_base_financiera\5 PRUEBAS SUSTANTIVAS\1 CAJA Y BANCOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE37739C-ABD9-4001-95B3-7F1C292EEC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E5CD2C-CF88-4B6D-89F2-5F768C87AC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Al 01/01/AAAA</t>
   </si>
   <si>
-    <t>DEL 01 DE ENERO AL 31  DE DICIEMBRE DE 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">AUDITORIA FINANCIERA </t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Entidad XXXXXXX</t>
+  </si>
+  <si>
+    <t>Del 01 de Enero al 31 de Diciembre de 2024</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +252,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,6 +493,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -506,13 +518,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1053,7 +1059,7 @@
   <dimension ref="B2:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,10 +1114,10 @@
       <c r="B5" s="9"/>
       <c r="C5" s="6"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="54"/>
+      <c r="E5" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="55"/>
       <c r="G5" s="10"/>
       <c r="H5" s="8"/>
       <c r="I5" s="11"/>
@@ -1121,10 +1127,10 @@
       <c r="B6" s="9"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="46"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="12" t="s">
@@ -1135,12 +1141,12 @@
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
+      <c r="D7" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="4"/>
       <c r="I7" s="12" t="s">
         <v>1</v>
@@ -1151,10 +1157,10 @@
       <c r="B8" s="9"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="55"/>
+      <c r="E8" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="47"/>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
       <c r="I8" s="12" t="s">
@@ -1166,10 +1172,10 @@
       <c r="B9" s="9"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="46"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="12" t="s">
@@ -1179,18 +1185,18 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="2:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="30"/>
       <c r="E11" s="31" t="s">
         <v>3</v>
@@ -1201,19 +1207,19 @@
       <c r="G11" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="51"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="32" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:11" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="38" t="s">
         <v>21</v>
       </c>
@@ -1238,8 +1244,8 @@
       <c r="K12"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="40"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
@@ -1528,16 +1534,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>